<commit_message>
Updated for 2024 Snake R returns
</commit_message>
<xml_diff>
--- a/DATA/Snake River Sockeye from Joint Staff Report.xlsx
+++ b/DATA/Snake River Sockeye from Joint Staff Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StiffH\Documents\Rcode\Osoyoos_recruits_SAR\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8669745E-8B0F-4848-8B13-014312BB4331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C7DC7B-2A39-4E71-BF49-DE199021DACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{155B2E9B-95A5-460C-8AF2-5BE6DDD194FF}"/>
+    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="13176" xr2:uid="{155B2E9B-95A5-460C-8AF2-5BE6DDD194FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Snake River Sockeye Estimates" sheetId="1" r:id="rId1"/>
@@ -175,58 +175,6 @@
           </rPr>
           <t xml:space="preserve">
 Lower Granite dam count only</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B46" authorId="1" shapeId="0" xr:uid="{119E01BE-5645-4C83-B19A-C93726D9FC24}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>DART - Ice Harbor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B47" authorId="1" shapeId="0" xr:uid="{33077813-A12A-40FB-9F1D-0B7794D3AEC1}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>DART - Ice Harbor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B48" authorId="1" shapeId="0" xr:uid="{4ADD0AF4-E6C1-4D8D-8FBA-D473F9A719CC}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>[hs] :</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-2269 at Ice Harbour [2024-02-28]</t>
         </r>
       </text>
     </comment>
@@ -396,9 +344,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -436,7 +384,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -542,7 +490,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -684,7 +632,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -692,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E239395F-5923-4EE8-BDFD-555D60C93601}">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B46" sqref="B46:B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1087,8 +1035,19 @@
         <v>1999</v>
       </c>
     </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>2024</v>
+      </c>
+      <c r="B49" s="4">
+        <v>1179</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;"Calibri"&amp;12&amp;K000000 Unclassified - Non-Classifié&amp;1#_x000D_</oddHeader>
+  </headerFooter>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>